<commit_message>
Part 1 dialogue update
Translated part 1 flavor text, diaries, endings.
</commit_message>
<xml_diff>
--- a/data/Map002.xlsx
+++ b/data/Map002.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Documents\GitHub\Captured-Als-To-Romeria-Translation\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16077AA6-F69A-4D28-9E9F-48F39A54B455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="160">
   <si>
     <t>リリーイベ</t>
   </si>
@@ -341,22 +347,325 @@
   </si>
   <si>
     <t xml:space="preserve">オーク2 </t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Oi!!
+One of the semen slaves has escaped, nyan!!
+Weren't you guys supposed to be on guard, nyaa?</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;Did you see them leaving?</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Are you listening!! Pig 1!! Pig 2!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Orc 2&gt;Oink... Oink…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\n&lt;Orc 1&gt;Oink, oink... </t>
+  </si>
+  <si>
+    <t>\n&lt;Orc 1&gt;Oiiink, snort.</t>
+  </si>
+  <si>
+    <t>\n&lt;Orc 1&gt;Oink, oink!</t>
+  </si>
+  <si>
+    <t>\n&lt;Orc 2&gt;Oink♥ Squoink♥</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;What is this! What's that attitude!
+I'm gonna turn you into jerky!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Don't look so happy!!
+Masochistic pigs!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Huh? I definitely locked it.
+100 percent, nya.
+This ain't my fault.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;Eh-…?</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Start looking, nya!
+No dinner until you find them, nya!</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;I'm the one who cooks their food though.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;I'm sorry.
+It's easy to get lost out in the woods.
+So don't stay out too late.</t>
+  </si>
+  <si>
+    <t>\n&lt;Orc 2&gt;Oink!</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Tsk.
+Worthless pigs.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;Shina…</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Hellooo. Anybody home-?</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;What are you talking about?
+I didn't come here to meet decent people.
+Rich people are rarely ever decent people.</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Excuuuse me! Helloooo!
+Anybody home-!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;\{A- NY- BO- DY-!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Guh...!!
+Wh-what the...!?
+A succubus...!?</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Shina!?
+Ako!! It's me, Ako!!
+Ako Ako Ako!!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Santa&gt;Don't come to me when you get captured and eaten.</t>
+  </si>
+  <si>
+    <t>\n&lt;Santa&gt;Hm? Do you know me?</t>
+  </si>
+  <si>
+    <t>\n&lt;Santa&gt;...Shina?</t>
+  </si>
+  <si>
+    <t>\n&lt;Santa&gt;Everyone was so worried that something had happened.
+Well, I suppose something did happen.
+What happened to you?</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Surprise attack!!
+Gotchaaa!!
+Who are you, nya!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Nyaaaan!?
+You're a succubus too!
+Why did you come here...</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Wait...
+Santa?</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Huh?
+Ako?
+What are you doing here, nya?</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;As if I'd just drop dead, nya!</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;Don't you call me Shinyan!
+I'll kill you!</t>
+  </si>
+  <si>
+    <t>\n&lt;Santa&gt;Stop this, Ako.
+This is Misty Mansion. I've heard rumors.
+There are no decent people living here.</t>
+  </si>
+  <si>
+    <t>\n&lt;Santa&gt;Ahaha. I didn't expect somebody even less decent
+than a rich person to come out.</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;(Although I profit a whole lot more.)</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;Ah, one more thing please.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;Stop...!
+So loud...! Keep it down!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Alright, alright.
+I got it.
+If anything looks good, I'll pick it up.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;We wrote everything down in this memo. Thanks again.
+I really appreciate it.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;B-but don't go out of your way.
+Only if you come across it.
+I don't want it that badly.</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Do you like that kind of thing, Lily?</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;Huh? What are you talking about?
+It's for research. As a succubus, I constantly have
+to keep informed about human tendencies.</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Hm.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;You're a succubus too. Stop obsessing over money,
+and drain at least one human.
+Honestly...</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Why are you getting so angry?</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;I'm not angry!
+Why are you giving me such a hard time?
+I think it's time for you to go. Take care now!</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Okaaaay.
+So everything on the memo, plus one romance novel!
+Bye bye!</t>
+  </si>
+  <si>
+    <t>\n&lt;Lily&gt;\{STOP SAYING THAT!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;Then, please get me these ingredients, Ako!
+Come back safe-♥</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Hey, hey.
+Why are you always making food for the humans?
+You're such a great cook.</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;That's all?</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;...?
+What do you mean... That's all?</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;If I cook tasty food, then the humans will stay healthy,
+and they'll give me better semen, no? The better their food
+is, the better they taste. I'm feeding myself too.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;Mmm... Pigs are really tasty too-!
+Deep fried tonkatsu... The oils and juices spreading
+through your mouth...</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;No, that's not what I meant...</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;It feels like my cheeks are about to melt♥
+I'm really gonna melt-♥
+Need some sauce too, oh, but first, salt and wasabi...</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;You don't suppose deep-fried human would taste good too?</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Oh, I meant to say!
+What if we were to open up a restaurant?
+We could make humans pay with their semen!</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;(I thought I might get through to Lime, but...
+Sure enough, I still sound crazy, believing
+humans and succubi could get along.)</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;That sounds great!
+I'd expect no less from Ako! You're so clever!</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Ahhh, back to the drawing board.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;But, do you think my cooking is really good enough
+that humans would sacrifice their own lives for it?</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Right? We'd all get good food, and we could all benefit one another!
+It's a win-win!
+Don't you think we could all get along?</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;No, no, Santa.
+We know each other...</t>
+  </si>
+  <si>
+    <t>\n&lt;Shina&gt;It's me, Shina, nya.
+Oh, right, of course.
+You wouldn't recognize me in this form.</t>
+  </si>
+  <si>
+    <t>\n&lt;Santa&gt;We stopped seeing you all of a sudden, but...
+I never imagined you had become a succubus...</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;I'm so glad you're safe...!
+I was so sure you were dead on the side of the road somewhere...</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Ahhhhh～...♥
+Shinyan is alive...
+I'm so glad...♥ Heh heh.</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;I'm bringing home some treasures too.
+Today is a win-win!
+Everybody profits in a successful business!</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;Romance? Like a romance novel?</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;So you're basically just fattening the humans up like pigs?</t>
+  </si>
+  <si>
+    <t>\n&lt;Ako&gt;You're creeping me out now!!</t>
+  </si>
+  <si>
+    <t>\n&lt;Orc 2&gt;Oink.
+Oink, squeal.</t>
+  </si>
+  <si>
+    <t>\n&lt;Lime&gt;Leave them alone-.
+This wouldn't have happened if you hadn't
+forgotten to lock the cell in the first place…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -364,28 +673,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -675,19 +1000,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:B84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.42578125" customWidth="1"/>
+    <col min="2" max="2" width="69.28515625" customWidth="1"/>
+    <col min="3" max="3" width="75.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -703,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -711,7 +1038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -719,7 +1046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -727,7 +1054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -735,615 +1062,843 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+      <c r="C62" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1351,7 +1906,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -1360,17 +1915,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>